<commit_message>
updated spreadsheet for VVSS lab 1
</commit_message>
<xml_diff>
--- a/VVSS/lab1/CheckLists/Lab01_ReviewReport.xlsx
+++ b/VVSS/lab1/CheckLists/Lab01_ReviewReport.xlsx
@@ -217,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -288,13 +288,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -377,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,16 +463,8 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -974,10 +959,10 @@
       <c r="C11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -989,7 +974,7 @@
       <c r="C12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -1004,7 +989,7 @@
       <c r="C13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="15" t="s">
@@ -1019,7 +1004,7 @@
       <c r="C14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -1034,7 +1019,7 @@
       <c r="C15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -1049,7 +1034,7 @@
       <c r="C16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -1064,7 +1049,7 @@
       <c r="C17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1190,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1219,22 +1204,22 @@
       <c r="E2" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8"/>
@@ -1489,7 +1474,9 @@
         <v>28</v>
       </c>
       <c r="D32" s="19"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="14" t="n">
+        <v>1.25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>